<commit_message>
AnsiString vypis_retezy_s_pouzitelnou_rozteci(double Rz,AnsiString separator=",",AnsiString total_separator=";",bool mm=false); - přídán poslední parametru zajišťující převod jednotek
přídání TmGrid knihovny
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -13,7 +13,6 @@
     <sheet name="rosta" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -141,9 +140,6 @@
   </si>
   <si>
     <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd</t>
-  </si>
-  <si>
-    <t>Globální aktualizace parametrů (RD, M, K, CT, P) objektů v kontinuálním režimu  z důvodu změny parametrů pohonu</t>
   </si>
   <si>
     <t>jedna volba ze 4 sloupců</t>
@@ -421,6 +417,9 @@
   </si>
   <si>
     <t>jedna volba ze 2 sloupců</t>
+  </si>
+  <si>
+    <t>Globální aktualizace parametrů (RD, M, K, CT, P) objektů v kontinuálním režimu  z důvodu změny parametrů pohonu aktuální rychlosti pohonu a rozestupu</t>
   </si>
 </sst>
 </file>
@@ -1064,54 +1063,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1126,24 +1077,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1166,12 +1099,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1193,12 +1120,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1210,33 +1131,72 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1255,7 +1215,46 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1751,13 +1750,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>95231</xdr:colOff>
+      <xdr:colOff>104756</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
@@ -1776,7 +1775,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2428875" y="1781175"/>
+          <a:off x="2438400" y="1857375"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2397,15 +2396,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>76183</xdr:colOff>
+      <xdr:colOff>85708</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>152382</xdr:rowOff>
+      <xdr:rowOff>161907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2422,7 +2421,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828925" y="2162175"/>
+          <a:off x="2838450" y="2247900"/>
           <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2435,13 +2434,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>95231</xdr:colOff>
+      <xdr:colOff>104756</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>171429</xdr:rowOff>
     </xdr:to>
@@ -2460,7 +2459,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2428875" y="2152650"/>
+          <a:off x="2438400" y="2228850"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4181,7 +4180,7 @@
   <dimension ref="B1:O11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:O3"/>
+      <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4192,45 +4191,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="G2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="H2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="J2" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4244,17 +4243,17 @@
       <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="61"/>
       <c r="N3" s="15"/>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -4267,58 +4266,58 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="19"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="61"/>
       <c r="N4" s="16"/>
       <c r="O4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="51" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="21"/>
+        <v>27</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="62"/>
       <c r="N5" s="17"/>
       <c r="O5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="29"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="21"/>
+        <v>27</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="62"/>
       <c r="N6" s="2" t="s">
         <v>12</v>
       </c>
@@ -4327,21 +4326,21 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="63"/>
       <c r="N7" s="2" t="s">
         <v>17</v>
       </c>
@@ -4354,7 +4353,7 @@
         <v>26</v>
       </c>
       <c r="O8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -4362,12 +4361,12 @@
         <v>39</v>
       </c>
       <c r="O9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -4377,27 +4376,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4424,112 +4423,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
-        <v>47</v>
+      <c r="B1" s="19" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="2:20" ht="113.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="70"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
       <c r="K3" s="15"/>
       <c r="L3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
+        <v>60</v>
+      </c>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="74"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
       <c r="K4" s="16"/>
-      <c r="L4" s="64" t="s">
-        <v>60</v>
+      <c r="L4" s="40" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="79"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="64" t="s">
-        <v>59</v>
+      <c r="D5" s="59"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="69"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="40" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="54"/>
-      <c r="C6" s="53" t="s">
+      <c r="B6" s="82"/>
+      <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="K6" s="10" t="s">
         <v>12</v>
       </c>
@@ -4538,57 +4537,57 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="54"/>
-      <c r="C7" s="53" t="s">
+      <c r="B7" s="82"/>
+      <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="79"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
       <c r="K7" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="91" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="B8" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="77"/>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="55"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="83"/>
+        <v>64</v>
+      </c>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4599,7 +4598,7 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -4608,20 +4607,11 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F15" s="50"/>
+      <c r="F15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
@@ -4629,7 +4619,16 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4644,7 +4643,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4653,24 +4652,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
-        <v>41</v>
+      <c r="B1" s="19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="103.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4681,22 +4680,22 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="61"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
@@ -4705,12 +4704,12 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
@@ -4719,15 +4718,15 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4738,7 +4737,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -4843,14 +4842,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
+      <c r="E9" s="89"/>
+      <c r="F9" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="90"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -4913,14 +4912,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33" t="s">
+      <c r="E15" s="90"/>
+      <c r="F15" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="33"/>
+      <c r="G15" s="91"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
Unit2 - nově, testování mGrid + možná bude PL_priority
TmGrid - aktualizace komentářů
aDoc a zadaní GAPO.xlsx aktulizace
TISPL.cpp resp. cbproj přidání Unit2
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
   <si>
     <t>TT Changes</t>
   </si>
@@ -421,9 +421,6 @@
     <t>jedna volba ze 2 sloupců</t>
   </si>
   <si>
-    <t>Globální aktualizace parametrů (RD, M, K, CT, P) objektů v kontinuálním režimu  z důvodu změny parametrů pohonu aktuální rychlosti pohonu a rozestupu</t>
-  </si>
-  <si>
     <t>RD,DD,M,P</t>
   </si>
   <si>
@@ -461,6 +458,12 @@
   </si>
   <si>
     <t>read-only + nedojde k přepoču</t>
+  </si>
+  <si>
+    <t>Globální aktualizace parametrů (RD, M, P) objektů v kontinuálním režimu  z důvodu změny parametrů pohonu aktuální rychlosti pohonu a rozestupu</t>
+  </si>
+  <si>
+    <t>možnost jednotlivé parametry  (šedé slopce) ještě rozdělit před změnou a po změně</t>
   </si>
 </sst>
 </file>
@@ -1277,143 +1280,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1435,6 +1303,141 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -5307,14 +5310,14 @@
       <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="53"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="77"/>
       <c r="N3" s="15"/>
       <c r="O3" t="s">
         <v>41</v>
@@ -5330,21 +5333,21 @@
       <c r="D4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="77"/>
       <c r="N4" s="16"/>
       <c r="O4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="67" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -5353,35 +5356,35 @@
       <c r="D5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="55"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="78"/>
       <c r="N5" s="17"/>
       <c r="O5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="78"/>
       <c r="N6" s="2" t="s">
         <v>12</v>
       </c>
@@ -5390,21 +5393,21 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="64"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="2" t="s">
         <v>17</v>
       </c>
@@ -5440,27 +5443,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5476,7 +5479,7 @@
   <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5527,8 +5530,8 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="58"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
       <c r="H3" s="43"/>
@@ -5565,34 +5568,34 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="98" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="83"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="89"/>
       <c r="K5" s="49"/>
       <c r="L5" s="40" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="65"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="83"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="89"/>
       <c r="K6" s="10" t="s">
         <v>12</v>
       </c>
@@ -5601,16 +5604,16 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="65"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="83"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="89"/>
       <c r="K7" s="10" t="s">
         <v>62</v>
       </c>
@@ -5619,33 +5622,33 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="92" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="75"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
       <c r="L8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="76"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="81"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="87"/>
       <c r="L9" t="s">
         <v>43</v>
       </c>
@@ -5675,6 +5678,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -5685,14 +5696,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5707,7 +5710,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5717,7 +5720,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="103.5" x14ac:dyDescent="0.25">
@@ -5744,22 +5747,22 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="77"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="67" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="100"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
@@ -5768,12 +5771,12 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="63"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="102"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
@@ -5782,12 +5785,12 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="64"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="104"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -5841,7 +5844,7 @@
   <sheetData>
     <row r="1" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="103.5" x14ac:dyDescent="0.25">
@@ -5852,13 +5855,13 @@
         <v>35</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="52" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>36</v>
@@ -5874,26 +5877,26 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="77"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="67" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
       <c r="I4" s="51" t="s">
         <v>12</v>
       </c>
@@ -5902,14 +5905,14 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="63"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="87"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="102"/>
       <c r="I5" s="51" t="s">
         <v>17</v>
       </c>
@@ -5918,14 +5921,14 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="64"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="89"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="104"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -5970,10 +5973,10 @@
   <sheetPr>
     <tabColor theme="3" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B1:O9"/>
+  <dimension ref="B1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5984,7 +5987,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="103.5" x14ac:dyDescent="0.25">
@@ -5995,40 +5998,40 @@
         <v>35</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="52" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="J2" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="100" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="100" t="s">
+      <c r="L2" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="100" t="s">
+      <c r="M2" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="100" t="s">
+      <c r="N2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="100" t="s">
+      <c r="O2" s="56" t="s">
         <v>76</v>
-      </c>
-      <c r="O2" s="101" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -6038,74 +6041,74 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="106"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="67" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="106"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="63"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="106"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="61"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="64"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="107"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="62"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
@@ -6114,15 +6117,20 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H8" s="99"/>
+      <c r="H8" s="54"/>
       <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H9" s="53"/>
+      <c r="I9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H9" s="98"/>
-      <c r="I9" t="s">
-        <v>79</v>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -6227,14 +6235,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="90" t="s">
+      <c r="D9" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91" t="s">
+      <c r="E9" s="109"/>
+      <c r="F9" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="91"/>
+      <c r="G9" s="110"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -6297,14 +6305,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="91"/>
-      <c r="F15" s="92" t="s">
+      <c r="E15" s="110"/>
+      <c r="F15" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="92"/>
+      <c r="G15" s="111"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
GAPO.xlsx - akutalizace gapoTT a gapoV - volba zda měnit Rx či R
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19110" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="17235" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
   <si>
     <t>TT Changes</t>
   </si>
@@ -99,9 +99,6 @@
     <t>režim</t>
   </si>
   <si>
-    <t>*šedě označené položky jsou zohledněny jenom pro KK</t>
-  </si>
-  <si>
     <t>KK</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd</t>
   </si>
   <si>
-    <t>jedna volba ze 4 sloupců</t>
-  </si>
-  <si>
     <t>nepřepínatelné, pouze ikona co zůstane a co se bude měnit (možná by bylo zavadějící)</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
   </si>
   <si>
     <t>Globální aktualizace parametrů pohonů a objektů v kontinuálním režimu  z důvodu změny parametrů vozíku</t>
-  </si>
-  <si>
-    <t>aRD, RD, M, Rz, Rx, K, CT, P</t>
   </si>
   <si>
     <t>aRD, RD, Rz, Rx, CT, DD, K</t>
@@ -240,85 +231,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">CT, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Rz, Rx, R</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>,M</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Rz, Rx, (R)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>, M, DD, P, CT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>aRD, RD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>, DD, CT</t>
-    </r>
-  </si>
-  <si>
     <t>M,P</t>
-  </si>
-  <si>
-    <t>aRD, RD, M, Rz, Rx, DD, P</t>
   </si>
   <si>
     <r>
@@ -460,17 +373,320 @@
     <t>možnost jednotlivé parametry  (šedé slopce) ještě rozdělit před změnou a po změně</t>
   </si>
   <si>
-    <t>pro všechny objekty se stejným pohonem  volba pouze v rámci daného dvousloupce (druhý dvousloupec je zakázaný)</t>
-  </si>
-  <si>
     <t>volba možná vždy, pokud je však z této skupiny voleno, musí být z této skupiny voleny všechny volby pro daný pohon, volby mohou být v rámci této dvouskupiny libovolné (samozřejmě párově propojené</t>
+  </si>
+  <si>
+    <t>pohon nepřiřazen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*šedě označené položky jsou zohledněny jenom pro KK či (mimo RD) pro pohon bez přiřazení </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CT, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rz, Rx, R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, M</t>
+    </r>
+  </si>
+  <si>
+    <t>pro všechny objekty se stejným pohonem  libovolnářádková volba pouze v rámci daného čtyřsloupce (dvousloupec je zakázaný)</t>
+  </si>
+  <si>
+    <t>pro všechny objekty se stejným pohonem  libovolná řádková volba pouze v rámci daného dvousloupce (čtyřsloupec je zakázaný)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rz,R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, M, DD, P, CT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rz, R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, M, DD, P, CT</t>
+    </r>
+  </si>
+  <si>
+    <t>jedna volba ze 6 sloupců (resp. 3 pro P3)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Rz, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rx!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, M, DD, P, CT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* položka označená </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rx!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tato volba bude možná pouze pokud Rx bude celočíselné!!!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aRD, RD, M, Rz, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rx!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, K, CT, P</t>
+    </r>
+  </si>
+  <si>
+    <t>aRD, RD, M, Rz, R, K, CT, P</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aRD, RD, M, Rz, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rx!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, DD, P</t>
+    </r>
+  </si>
+  <si>
+    <t>aRD, RD, M, Rz, R, DD, P</t>
+  </si>
+  <si>
+    <t>DD, R</t>
+  </si>
+  <si>
+    <t>DD, Rx</t>
+  </si>
+  <si>
+    <t>K, CT, R</t>
+  </si>
+  <si>
+    <t>K, CT, Rx</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aRD, RD, R, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> K</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aRD, RD, Rz, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> K</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>aRD, RD, R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>,  DD, CT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">aRD, RD, Rz, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> DD, CT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +768,57 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -603,7 +870,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1151,11 +1418,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,6 +1655,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1315,12 +1673,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1328,9 +1680,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1436,6 +1785,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1564,13 +1974,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>22006</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>222031</xdr:rowOff>
@@ -1672,13 +2082,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>656</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>22663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>181631</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>222688</xdr:rowOff>
@@ -1744,15 +2154,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>129409</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>14780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>319909</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>24305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1780,15 +2190,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>327134</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>15437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>508109</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>24962</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1968,15 +2378,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>314308</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>171432</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2006,16 +2416,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>514331</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>190479</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2032,7 +2442,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4857750" y="2752725"/>
+          <a:off x="4857750" y="3009900"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2120,13 +2530,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
@@ -2158,13 +2568,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
@@ -2196,13 +2606,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
@@ -2234,13 +2644,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
@@ -2272,13 +2682,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
@@ -2336,7 +2746,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3228975" y="2152650"/>
+          <a:off x="3228975" y="2228850"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2641,6 +3051,599 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2438400" y="2228850"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Obrázek 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2609850" y="2628900"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66658</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Obrázek 34"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3419475" y="2628900"/>
+          <a:ext cx="133333" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>16094</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Obrázek 35"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="225644"/>
+          <a:ext cx="190500" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>192470</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14452</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="183931" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Obrázek 36"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3278570" y="224002"/>
+          <a:ext cx="183931" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Obrázek 37"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="1666875"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Obrázek 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="1857375"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Obrázek 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2228850"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Obrázek 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2419350"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Obrázek 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2047875"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85706</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Obrázek 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4219575" y="2619375"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22006</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Obrázek 43"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="231556"/>
+          <a:ext cx="190500" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>656</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22663</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="180975" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Obrázek 44"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486931" y="232213"/>
+          <a:ext cx="180975" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Obrázek 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="2428875"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Obrázek 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="1666875"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Obrázek 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="1857375"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Obrázek 48"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="2238375"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Obrázek 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="2057400"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2729,13 +3732,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>20692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>220717</xdr:rowOff>
@@ -2837,13 +3840,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>1970</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>185901</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
@@ -2949,13 +3952,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
@@ -3053,7 +4056,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -3086,13 +4089,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>129409</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>14780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>319909</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>24305</xdr:rowOff>
@@ -3122,13 +4125,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>327134</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>15437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>508109</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>24962</xdr:rowOff>
@@ -3158,13 +4161,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>314308</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>180957</xdr:rowOff>
@@ -3196,13 +4199,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>514331</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
@@ -3235,19 +4238,133 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66656</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Obrázek 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="2505075"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
       <xdr:row>4</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Obrázek 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152775" y="2505075"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85708</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Obrázek 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1581150" y="2257425"/>
+          <a:ext cx="133333" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66656</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Obrázek 31"/>
+        <xdr:cNvPr id="35" name="Obrázek 34"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3260,7 +4377,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1952625" y="2047875"/>
+          <a:off x="1943100" y="2705100"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3270,6 +4387,480 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Obrázek 35"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152775" y="2705100"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66656</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Obrázek 37"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="2895600"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Obrázek 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152775" y="2895600"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="133333" cy="142857"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Obrázek 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1962150" y="2647950"/>
+          <a:ext cx="133333" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Obrázek 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="2247900"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="133333" cy="142857"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Obrázek 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2371725" y="2828925"/>
+          <a:ext cx="133333" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Obrázek 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952625" y="2438400"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Obrázek 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1571625" y="2714625"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20692</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Obrázek 40"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="230242"/>
+          <a:ext cx="190500" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1970</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="183931" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Obrázek 44"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3230945" y="228600"/>
+          <a:ext cx="183931" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17079</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Obrázek 47"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1847850" y="226629"/>
+          <a:ext cx="190500" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5912</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>16422</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="183931" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Obrázek 48"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2034737" y="225972"/>
+          <a:ext cx="183931" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85706</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Obrázek 79"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="2133600"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Obrázek 80"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="2324100"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -3285,7 +4876,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Obrázek 32"/>
+        <xdr:cNvPr id="82" name="Obrázek 81"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3298,83 +4889,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2047875"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85708</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>180957</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Obrázek 33"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1581150" y="2257425"/>
-          <a:ext cx="133333" cy="142857"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9504</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Obrázek 34"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1952625" y="2247900"/>
+          <a:off x="2362200" y="2514600"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3399,7 +4914,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Obrázek 35"/>
+        <xdr:cNvPr id="83" name="Obrázek 82"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3412,45 +4927,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2247900"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9504</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Obrázek 37"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1952625" y="2438400"/>
+          <a:off x="2362200" y="2714625"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3475,7 +4952,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Obrázek 38"/>
+        <xdr:cNvPr id="84" name="Obrázek 83"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3488,7 +4965,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2438400"/>
+          <a:off x="2362200" y="2905125"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3498,39 +4975,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="133333" cy="142857"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Obrázek 39"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1962150" y="2647950"/>
-          <a:ext cx="133333" cy="142857"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -3541,7 +4985,7 @@
     <xdr:ext cx="152381" cy="171429"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Obrázek 41"/>
+        <xdr:cNvPr id="85" name="Obrázek 84"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3554,7 +4998,225 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2247900"/>
+          <a:off x="2362200" y="3095625"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="86" name="Obrázek 85"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2124075"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="87" name="Obrázek 86"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2314575"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="88" name="Obrázek 87"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2505075"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="Obrázek 88"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2705100"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="Obrázek 89"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2895600"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="Obrázek 90"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="3086100"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3569,26 +5231,26 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="133333" cy="142857"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Obrázek 42"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2371725" y="2828925"/>
-          <a:ext cx="133333" cy="142857"/>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="Obrázek 91"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2371725" y="3276600"/>
+          <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3599,15 +5261,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="Obrázek 43"/>
+        <xdr:cNvPr id="93" name="Obrázek 92"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3620,40 +5282,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1952625" y="2438400"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="152381" cy="171429"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Obrázek 46"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1571625" y="2714625"/>
+          <a:off x="2762250" y="3267075"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5135,25 +6764,25 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:O11"/>
+  <dimension ref="B1:S13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="5" max="12" width="3" customWidth="1"/>
+    <col min="5" max="16" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
@@ -5164,34 +6793,46 @@
         <v>25</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>52</v>
+        <v>81</v>
+      </c>
+      <c r="J2" s="122" t="s">
+        <v>91</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>29</v>
+        <v>78</v>
+      </c>
+      <c r="L2" s="122" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
@@ -5199,22 +6840,26 @@
         <v>20</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="67"/>
+        <v>26</v>
+      </c>
+      <c r="E3" s="69"/>
       <c r="F3" s="73"/>
-      <c r="G3" s="67"/>
+      <c r="G3" s="69"/>
       <c r="H3" s="73"/>
-      <c r="I3" s="67"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="73"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
-      <c r="N3" s="15"/>
-      <c r="O3" t="s">
-        <v>40</v>
+      <c r="K3" s="69"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
+      <c r="R3" s="15"/>
+      <c r="S3" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
@@ -5222,118 +6867,175 @@
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="67"/>
+        <v>26</v>
+      </c>
+      <c r="E4" s="69"/>
       <c r="F4" s="73"/>
-      <c r="G4" s="67"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="67"/>
+      <c r="I4" s="69"/>
       <c r="J4" s="73"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="68"/>
-      <c r="N4" s="16"/>
-      <c r="O4" t="s">
-        <v>79</v>
+      <c r="K4" s="69"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="70"/>
+      <c r="R4" s="16"/>
+      <c r="S4" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="74"/>
       <c r="F5" s="75"/>
       <c r="G5" s="74"/>
       <c r="H5" s="75"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="70"/>
-      <c r="N5" s="17"/>
-      <c r="O5" t="s">
-        <v>79</v>
+      <c r="I5" s="71"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="72"/>
+      <c r="R5" s="17"/>
+      <c r="S5" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="78"/>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="77"/>
       <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="74"/>
       <c r="F6" s="75"/>
       <c r="G6" s="74"/>
       <c r="H6" s="75"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="70"/>
-      <c r="N6" s="2" t="s">
+      <c r="I6" s="71"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="72"/>
+      <c r="R6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O6" t="s">
+      <c r="S6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="77"/>
+      <c r="C7" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="113"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="126"/>
+      <c r="R7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="79"/>
-      <c r="C7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="72"/>
-      <c r="N7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" t="s">
+    <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="116"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="120"/>
+      <c r="R8" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="111" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>32</v>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="127" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="30">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="M8:P8"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5350,11 +7052,11 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5367,25 +7069,25 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:T15"/>
+  <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="4" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="4" max="13" width="3" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="113.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
@@ -5393,54 +7095,70 @@
         <v>19</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="67"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="73"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
-      <c r="K3" s="15"/>
-      <c r="L3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="44"/>
+      <c r="O3" s="15"/>
+      <c r="P3" t="s">
+        <v>51</v>
+      </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="40"/>
       <c r="S3" s="40"/>
       <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
@@ -5451,134 +7169,175 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="40" t="s">
-        <v>57</v>
+      <c r="H4" s="130"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="48"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="40" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="86" t="s">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="85" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="96"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="40" t="s">
-        <v>80</v>
+      <c r="D5" s="71"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="95"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="40" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="86"/>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="85"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="96"/>
-      <c r="K6" s="10" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="95"/>
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
-        <v>30</v>
+      <c r="P6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="86"/>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="85"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="96"/>
-      <c r="K7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="D7" s="71"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="95"/>
+      <c r="O7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87"/>
+      <c r="P8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="80"/>
+      <c r="C9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="88"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="93"/>
+      <c r="P9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="88"/>
-      <c r="L8" t="s">
-        <v>41</v>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="127" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="81"/>
-      <c r="C9" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="89"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="94"/>
-      <c r="L9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F15" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
+  <mergeCells count="30">
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
@@ -5612,30 +7371,30 @@
   <sheetData>
     <row r="1" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>35</v>
-      </c>
       <c r="I2" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -5645,77 +7404,77 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="100"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="99"/>
       <c r="I4" s="51" t="s">
         <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="101"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="101"/>
       <c r="I5" s="51" t="s">
         <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="79"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="104"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="103"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5754,24 +7513,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>36</v>
-      </c>
       <c r="G2" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -5781,69 +7540,69 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="101"/>
-      <c r="E5" s="102"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="101"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="79"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="103"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5878,51 +7637,51 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="H2" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="M2" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" s="55" t="s">
-        <v>73</v>
-      </c>
       <c r="O2" s="56" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -5932,10 +7691,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -5946,16 +7705,16 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="100"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="99"/>
       <c r="H4" s="57"/>
       <c r="I4" s="59"/>
       <c r="J4" s="64"/>
@@ -5966,14 +7725,14 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="101"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="63"/>
       <c r="I5" s="59"/>
       <c r="J5" s="58"/>
@@ -5984,14 +7743,14 @@
       <c r="O5" s="61"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="79"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="104"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="103"/>
       <c r="H6" s="65"/>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -6004,24 +7763,24 @@
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="H7" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H8" s="54"/>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H9" s="53"/>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -6126,14 +7885,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="109"/>
-      <c r="F9" s="110" t="s">
+      <c r="E9" s="108"/>
+      <c r="F9" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="110"/>
+      <c r="G9" s="109"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -6196,14 +7955,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="110"/>
-      <c r="F15" s="111" t="s">
+      <c r="E15" s="109"/>
+      <c r="F15" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="111"/>
+      <c r="G15" s="110"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
GAPO.xlsx - aktualizace zadání gapoTT, pohon, který nebude přiřazen k objektům nebude mít poslední sloupec (resp. nebude tam mít checkbox/radio)
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -820,7 +820,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -869,8 +869,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1419,6 +1425,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1434,19 +1449,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1503,11 +1505,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1797,19 +1810,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1846,6 +1856,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3363,44 +3379,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>85706</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Obrázek 42"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4219575" y="2619375"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
@@ -6767,7 +6745,7 @@
   <dimension ref="B1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:P3"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6807,13 +6785,13 @@
       <c r="I2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="122" t="s">
+      <c r="J2" s="121" t="s">
         <v>91</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="122" t="s">
+      <c r="L2" s="121" t="s">
         <v>92</v>
       </c>
       <c r="M2" s="25" t="s">
@@ -6940,7 +6918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="77"/>
       <c r="C7" s="112" t="s">
         <v>24</v>
@@ -6952,14 +6930,14 @@
       <c r="F7" s="114"/>
       <c r="G7" s="113"/>
       <c r="H7" s="114"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="126"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="125"/>
       <c r="R7" s="2" t="s">
         <v>17</v>
       </c>
@@ -6978,15 +6956,15 @@
       <c r="E8" s="118"/>
       <c r="F8" s="119"/>
       <c r="G8" s="119"/>
-      <c r="H8" s="121"/>
+      <c r="H8" s="120"/>
       <c r="I8" s="118"/>
       <c r="J8" s="119"/>
       <c r="K8" s="119"/>
       <c r="L8" s="119"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="120"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="134"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
       <c r="R8" s="68" t="s">
         <v>52</v>
       </c>
@@ -7021,7 +6999,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="126" t="s">
         <v>82</v>
       </c>
     </row>
@@ -7139,10 +7117,10 @@
       <c r="E3" s="73"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="128"/>
       <c r="L3" s="43"/>
       <c r="M3" s="44"/>
       <c r="O3" s="15"/>
@@ -7169,8 +7147,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="131"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="130"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7233,10 +7211,10 @@
       <c r="E7" s="76"/>
       <c r="F7" s="96"/>
       <c r="G7" s="97"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="133"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="131"/>
+      <c r="K7" s="132"/>
       <c r="L7" s="94"/>
       <c r="M7" s="95"/>
       <c r="O7" s="10" t="s">
@@ -7307,7 +7285,7 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="127" t="s">
+      <c r="B14" s="126" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GAPO.xlsx - ještě update
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -876,7 +876,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1458,6 +1458,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1520,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1816,21 +1829,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1852,13 +1870,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3116,14 +3134,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>141633</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66658</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>74940</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>161907</xdr:rowOff>
     </xdr:to>
@@ -3142,8 +3160,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3419475" y="2628900"/>
-          <a:ext cx="133333" cy="142857"/>
+          <a:off x="3231046" y="2636354"/>
+          <a:ext cx="132090" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3623,6 +3641,44 @@
         <a:xfrm>
           <a:off x="4010025" y="2057400"/>
           <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85706</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>183025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Obrázek 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3620328" y="2628900"/>
+          <a:ext cx="151139" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6785,13 +6841,13 @@
       <c r="I2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="121" t="s">
+      <c r="J2" s="123" t="s">
         <v>91</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="121" t="s">
+      <c r="L2" s="123" t="s">
         <v>92</v>
       </c>
       <c r="M2" s="25" t="s">
@@ -6930,14 +6986,14 @@
       <c r="F7" s="114"/>
       <c r="G7" s="113"/>
       <c r="H7" s="114"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="122"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="122"/>
-      <c r="P7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="127"/>
+      <c r="N7" s="127"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="128"/>
       <c r="R7" s="2" t="s">
         <v>17</v>
       </c>
@@ -6956,15 +7012,15 @@
       <c r="E8" s="118"/>
       <c r="F8" s="119"/>
       <c r="G8" s="119"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="133"/>
-      <c r="N8" s="134"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="136"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="137"/>
       <c r="R8" s="68" t="s">
         <v>52</v>
       </c>
@@ -6999,7 +7055,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="126" t="s">
+      <c r="B13" s="129" t="s">
         <v>82</v>
       </c>
     </row>
@@ -7011,8 +7067,8 @@
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="E8:H8"/>
-    <mergeCell ref="I8:L8"/>
     <mergeCell ref="M8:P8"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="E3:F3"/>
@@ -7117,10 +7173,10 @@
       <c r="E3" s="73"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="128"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
       <c r="L3" s="43"/>
       <c r="M3" s="44"/>
       <c r="O3" s="15"/>
@@ -7147,8 +7203,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="130"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="133"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7211,10 +7267,10 @@
       <c r="E7" s="76"/>
       <c r="F7" s="96"/>
       <c r="G7" s="97"/>
-      <c r="H7" s="131"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="132"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="135"/>
       <c r="L7" s="94"/>
       <c r="M7" s="95"/>
       <c r="O7" s="10" t="s">
@@ -7285,7 +7341,7 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="129" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GAPO.xlsx - aktualizace gapoR - zakomponování i S&G objektu (mění se mu CT)
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="98">
   <si>
     <t>TT Changes</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>*změny proběhnou pouze v případě změny aRD a Rz (pouze v případě Rx,R se pro daný pohon nic neděje)</t>
-  </si>
-  <si>
-    <t>*S&amp;G režim se nezohledňuje, pouze ve validaci zda se stíhá přejezd</t>
   </si>
   <si>
     <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd</t>
@@ -680,6 +677,18 @@
       </rPr>
       <t xml:space="preserve"> DD, CT</t>
     </r>
+  </si>
+  <si>
+    <t>*S&amp;G režim se zohledňuje přímo výpočtem (není možná volba), pouze ve validaci zda se stíhá přejezd</t>
+  </si>
+  <si>
+    <t>S&amp;G</t>
+  </si>
+  <si>
+    <t>není jiné volby</t>
+  </si>
+  <si>
+    <t>O8</t>
   </si>
 </sst>
 </file>
@@ -820,7 +829,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -871,12 +880,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -1529,11 +1544,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1681,6 +1746,15 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1876,11 +1950,30 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2190,14 +2283,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>129409</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>14780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>319909</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>24305</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16022</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2226,14 +2319,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>327134</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>15437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>508109</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>24962</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2338,13 +2431,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>85708</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>161907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2376,13 +2469,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>104756</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2413,14 +2506,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>164409</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>314308</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>297742</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>171432</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2438,7 +2531,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4676775" y="2762250"/>
+          <a:off x="5456996" y="3250510"/>
           <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2452,13 +2545,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>514331</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2528,13 +2621,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95231</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2604,44 +2697,6 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>85706</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Obrázek 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3619500" y="1781175"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -2653,6 +2708,44 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Obrázek 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3619500" y="1781175"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85706</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="Obrázek 21"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -2667,6 +2760,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3619500" y="2162175"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85706</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Obrázek 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3619500" y="2352675"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2681,50 +2812,12 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Obrázek 22"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3619500" y="2352675"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>85706</xdr:colOff>
-      <xdr:row>4</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2756,13 +2849,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95231</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>171429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2781,6 +2874,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3228975" y="2228850"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95231</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Obrázek 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2343150"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2795,50 +2926,12 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95231</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171429</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Obrázek 25"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3228975" y="2343150"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95231</xdr:colOff>
-      <xdr:row>4</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2858,6 +2951,120 @@
         <a:xfrm>
           <a:off x="3228975" y="1971675"/>
           <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76183</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Obrázek 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828925" y="2371725"/>
+          <a:ext cx="133333" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>104756</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Obrázek 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="2352675"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95233</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Obrázek 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="1981200"/>
+          <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2871,17 +3078,55 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>76183</xdr:colOff>
+      <xdr:colOff>95231</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171432</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Obrázek 27"/>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Obrázek 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828925" y="1971675"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85708</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Obrázek 31"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2894,7 +3139,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828925" y="2371725"/>
+          <a:off x="2838450" y="2247900"/>
           <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2908,165 +3153,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>104756</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Obrázek 28"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2438400" y="2352675"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95233</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161907</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Obrázek 29"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2447925" y="1981200"/>
-          <a:ext cx="133333" cy="142857"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>95231</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Obrázek 30"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2828925" y="1971675"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85708</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161907</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Obrázek 31"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2838450" y="2247900"/>
-          <a:ext cx="133333" cy="142857"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>104756</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>171429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3098,13 +3191,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3136,13 +3229,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>141633</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>74940</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>161907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3269,7 +3362,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
@@ -3302,7 +3395,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
@@ -3322,6 +3415,39 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3228975" y="2228850"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Obrázek 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2419350"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3336,39 +3462,6 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="152381" cy="171429"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Obrázek 40"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3228975" y="2419350"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>4</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
@@ -3463,13 +3556,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>180954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3539,44 +3632,6 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Obrázek 47"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4010025" y="1857375"/>
-          <a:ext cx="152381" cy="171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -3588,6 +3643,44 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Obrázek 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="1857375"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76181</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="49" name="Obrázek 48"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -3615,13 +3708,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3653,13 +3746,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>11596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>183025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3687,6 +3780,77 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>153642</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>26504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>86950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>169361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Obrázek 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="2445026"/>
+          <a:ext cx="132090" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>153642</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>26504</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="132090" cy="142857"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Obrázek 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="2834308"/>
+          <a:ext cx="132090" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6798,10 +6962,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:S13"/>
+  <dimension ref="B1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,47 +6991,47 @@
         <v>25</v>
       </c>
       <c r="E2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>47</v>
-      </c>
       <c r="H2" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="123" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="126" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="126" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="M2" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="123" t="s">
-        <v>92</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N2" s="25" t="s">
+      <c r="P2" s="27" t="s">
         <v>93</v>
-      </c>
-      <c r="O2" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="27" t="s">
-        <v>94</v>
       </c>
       <c r="R2" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="146" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -6876,221 +7040,293 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="70"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="73"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>12</v>
-      </c>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="80"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="70"/>
+        <v>95</v>
+      </c>
+      <c r="E4" s="143"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="142"/>
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="147"/>
+      <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="72"/>
+      <c r="D5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="67"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="69"/>
       <c r="R5" s="17"/>
       <c r="S5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="77"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="71"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="72"/>
       <c r="J6" s="76"/>
-      <c r="K6" s="71"/>
+      <c r="K6" s="72"/>
       <c r="L6" s="76"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="72"/>
-      <c r="R6" s="2" t="s">
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="73"/>
+      <c r="R6" s="145"/>
+      <c r="S6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="75"/>
+      <c r="R7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S7" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="77"/>
-      <c r="C7" s="112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="113"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="128"/>
-      <c r="R7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="115" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="117" t="s">
+      <c r="B8" s="80"/>
+      <c r="C8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="77"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="75"/>
+      <c r="R8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="80"/>
+      <c r="C9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="143"/>
+      <c r="F9" s="144"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="142"/>
+      <c r="I9" s="142"/>
+      <c r="J9" s="142"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="142"/>
+      <c r="N9" s="142"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="142"/>
+      <c r="R9" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="80"/>
+      <c r="C10" s="115" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="F10" s="117"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="131"/>
+      <c r="S10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="118" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="118"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="136"/>
-      <c r="N8" s="137"/>
-      <c r="O8" s="137"/>
-      <c r="P8" s="137"/>
-      <c r="R8" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="111" t="s">
-        <v>74</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="D11" s="119"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="127"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="139"/>
+      <c r="N11" s="140"/>
+      <c r="O11" s="140"/>
+      <c r="P11" s="140"/>
+      <c r="S11" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="S10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>31</v>
+      <c r="B12" s="114" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="129" t="s">
-        <v>82</v>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="132" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="35">
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="K8:L8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7118,7 +7354,7 @@
   <sheetData>
     <row r="1" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="2:24" ht="150" customHeight="1" x14ac:dyDescent="0.25">
@@ -7129,34 +7365,34 @@
         <v>19</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="I2" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="J2" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="K2" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="M2" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>28</v>
@@ -7169,19 +7405,19 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="73"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="76"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="131"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="134"/>
       <c r="L3" s="43"/>
       <c r="M3" s="44"/>
       <c r="O3" s="15"/>
       <c r="P3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="40"/>
@@ -7203,54 +7439,54 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="133"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="136"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
       <c r="M4" s="48"/>
       <c r="O4" s="16"/>
       <c r="P4" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="88" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="95"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="98"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="85"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="98"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7259,65 +7495,65 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="85"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="95"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="98"/>
       <c r="O7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="79" t="s">
-        <v>52</v>
+      <c r="B8" s="82" t="s">
+        <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="81"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="87"/>
+        <v>53</v>
+      </c>
+      <c r="D8" s="84"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="90"/>
       <c r="P8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="80"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="88"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="91"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="93"/>
+        <v>54</v>
+      </c>
+      <c r="D9" s="91"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="95"/>
+      <c r="M9" s="96"/>
       <c r="P9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
@@ -7327,12 +7563,12 @@
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
@@ -7341,8 +7577,8 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="129" t="s">
-        <v>82</v>
+      <c r="B14" s="132" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
@@ -7405,24 +7641,24 @@
   <sheetData>
     <row r="1" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>34</v>
@@ -7438,26 +7674,26 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="80" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="99"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="102"/>
       <c r="I4" s="51" t="s">
         <v>12</v>
       </c>
@@ -7466,14 +7702,14 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="101"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="104"/>
       <c r="I5" s="51" t="s">
         <v>17</v>
       </c>
@@ -7482,14 +7718,14 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="78"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="103"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -7498,12 +7734,12 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -7547,12 +7783,12 @@
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>33</v>
@@ -7574,22 +7810,22 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="80" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="102"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
@@ -7598,12 +7834,12 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
@@ -7612,12 +7848,12 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="78"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -7626,12 +7862,12 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -7671,51 +7907,51 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="103.5" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="55" t="s">
         <v>61</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>62</v>
       </c>
       <c r="J2" s="55" t="s">
         <v>34</v>
       </c>
       <c r="K2" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="M2" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="N2" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="O2" s="56" t="s">
         <v>66</v>
-      </c>
-      <c r="O2" s="56" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -7725,10 +7961,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -7739,16 +7975,16 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="80" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="99"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="102"/>
       <c r="H4" s="57"/>
       <c r="I4" s="59"/>
       <c r="J4" s="64"/>
@@ -7759,14 +7995,14 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="101"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="104"/>
       <c r="H5" s="63"/>
       <c r="I5" s="59"/>
       <c r="J5" s="58"/>
@@ -7777,14 +8013,14 @@
       <c r="O5" s="61"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="78"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="103"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
       <c r="H6" s="65"/>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -7803,18 +8039,18 @@
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H8" s="54"/>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H9" s="53"/>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -7919,14 +8155,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="108" t="s">
+      <c r="D9" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="108"/>
-      <c r="F9" s="109" t="s">
+      <c r="E9" s="111"/>
+      <c r="F9" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="109"/>
+      <c r="G9" s="112"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -7989,14 +8225,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="109" t="s">
+      <c r="D15" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="109"/>
-      <c r="F15" s="110" t="s">
+      <c r="E15" s="112"/>
+      <c r="F15" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="110"/>
+      <c r="G15" s="113"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
gapo.xlsx - grafický fix
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="17235" windowHeight="7650"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="17235" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
   <si>
     <t>TT Changes</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>O8</t>
+  </si>
+  <si>
+    <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd a jedostatečný mezerový fond</t>
   </si>
 </sst>
 </file>
@@ -4438,13 +4441,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66656</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
+      <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4461,7 +4464,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1943100" y="2505075"/>
+          <a:off x="1943100" y="2514600"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4476,13 +4479,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
+      <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4499,7 +4502,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3152775" y="2505075"/>
+          <a:off x="3152775" y="2514600"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4702,9 +4705,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="133333" cy="142857"/>
     <xdr:pic>
@@ -4722,7 +4725,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1962150" y="2647950"/>
+          <a:off x="1952625" y="3095625"/>
           <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4735,9 +4738,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
     <xdr:pic>
@@ -4755,7 +4758,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2247900"/>
+          <a:off x="3152775" y="3086100"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4768,9 +4771,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="133333" cy="142857"/>
     <xdr:pic>
@@ -4788,7 +4791,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="2828925"/>
+          <a:off x="3162300" y="3286125"/>
           <a:ext cx="133333" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4801,9 +4804,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
     <xdr:pic>
@@ -4821,7 +4824,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1952625" y="2438400"/>
+          <a:off x="1943100" y="3257550"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5064,13 +5067,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>85706</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190479</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9504</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5087,7 +5090,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="2514600"/>
+          <a:off x="2362200" y="2524125"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5282,13 +5285,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>76181</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180954</xdr:rowOff>
+      <xdr:rowOff>190479</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5305,7 +5308,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2752725" y="2505075"/>
+          <a:off x="2752725" y="2514600"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5427,7 +5430,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
@@ -5447,7 +5450,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="3276600"/>
+          <a:off x="2362200" y="3276600"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5460,7 +5463,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -5480,7 +5483,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2762250" y="3267075"/>
+          <a:off x="2752725" y="3267075"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6964,7 +6967,7 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
@@ -7341,8 +7344,8 @@
   </sheetPr>
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7630,7 +7633,7 @@
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7734,7 +7737,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
formy GAPO, aktualizace colcount nahrazeno za rowconut u tvorbu dynamického pole objektů objekty
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="17235" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="obecné rozšíř. o výpis param. " sheetId="5" r:id="rId5"/>
     <sheet name="rosta" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1764,193 +1764,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1959,24 +1837,146 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2891,13 +2891,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>8283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95231</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>171429</xdr:rowOff>
+      <xdr:rowOff>179712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2914,8 +2914,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3228975" y="2343150"/>
-          <a:ext cx="152381" cy="171429"/>
+          <a:off x="3232288" y="3031435"/>
+          <a:ext cx="151139" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3432,7 +3432,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>8283</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152381" cy="171429"/>
     <xdr:pic>
@@ -3450,7 +3450,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3228975" y="2419350"/>
+          <a:off x="3629853" y="3031435"/>
           <a:ext cx="152381" cy="171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6967,8 +6967,8 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7008,13 +7008,13 @@
       <c r="I2" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="126" t="s">
+      <c r="J2" s="76" t="s">
         <v>90</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="126" t="s">
+      <c r="L2" s="76" t="s">
         <v>91</v>
       </c>
       <c r="M2" s="25" t="s">
@@ -7034,7 +7034,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="106" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7043,50 +7043,50 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="76"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="73"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="108"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="80"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="143"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="142"/>
-      <c r="I4" s="142"/>
-      <c r="J4" s="142"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="142"/>
-      <c r="M4" s="142"/>
-      <c r="N4" s="142"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="147"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7120,25 +7120,25 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="72"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="76"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="73"/>
-      <c r="R6" s="145"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="108"/>
+      <c r="R6" s="82"/>
       <c r="S6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7147,18 +7147,18 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="79"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="86"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="75"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="109"/>
       <c r="R7" s="2" t="s">
         <v>12</v>
       </c>
@@ -7167,25 +7167,25 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="79"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="75"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="109"/>
       <c r="R8" s="2" t="s">
         <v>17</v>
       </c>
@@ -7194,25 +7194,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="80"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="144"/>
-      <c r="G9" s="141"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="142"/>
-      <c r="L9" s="142"/>
-      <c r="M9" s="142"/>
-      <c r="N9" s="142"/>
-      <c r="O9" s="142"/>
-      <c r="P9" s="142"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
       <c r="R9" s="71" t="s">
         <v>51</v>
       </c>
@@ -7221,55 +7221,55 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="80"/>
-      <c r="C10" s="115" t="s">
+      <c r="B10" s="101"/>
+      <c r="C10" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="116"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="116"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="131"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="110"/>
       <c r="S10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="125"/>
-      <c r="J11" s="127"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="139"/>
-      <c r="N11" s="140"/>
-      <c r="O11" s="140"/>
-      <c r="P11" s="140"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
       <c r="S11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="72" t="s">
         <v>73</v>
       </c>
     </row>
@@ -7289,24 +7289,12 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="132" t="s">
+      <c r="B16" s="79" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:P4"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="M11:P11"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E6:F6"/>
@@ -7315,19 +7303,31 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="M11:P11"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="O3:P3"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="O10:P10"/>
   </mergeCells>
@@ -7344,8 +7344,8 @@
   </sheetPr>
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7408,14 +7408,14 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="76"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="134"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="81"/>
       <c r="L3" s="43"/>
       <c r="M3" s="44"/>
       <c r="O3" s="15"/>
@@ -7442,8 +7442,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="136"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="114"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7454,42 +7454,42 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="133" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="98"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="128"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="98"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7498,20 +7498,20 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="128"/>
       <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
@@ -7520,41 +7520,41 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="129" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="90"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="120"/>
       <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="83"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="91"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="96"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="126"/>
       <c r="P9" t="s">
         <v>39</v>
       </c>
@@ -7580,7 +7580,7 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="79" t="s">
         <v>81</v>
       </c>
     </row>
@@ -7589,12 +7589,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7611,14 +7613,12 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7677,26 +7677,26 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="108"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="102"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="138"/>
       <c r="I4" s="51" t="s">
         <v>12</v>
       </c>
@@ -7705,14 +7705,14 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="104"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="141"/>
       <c r="I5" s="51" t="s">
         <v>17</v>
       </c>
@@ -7721,14 +7721,14 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="144"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -7813,22 +7813,22 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="108"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="138"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
@@ -7837,12 +7837,12 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="141"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
@@ -7851,12 +7851,12 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="106"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="144"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -7964,10 +7964,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="108"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -7978,16 +7978,16 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="102"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="138"/>
       <c r="H4" s="57"/>
       <c r="I4" s="59"/>
       <c r="J4" s="64"/>
@@ -7998,14 +7998,14 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="104"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="141"/>
       <c r="H5" s="63"/>
       <c r="I5" s="59"/>
       <c r="J5" s="58"/>
@@ -8016,14 +8016,14 @@
       <c r="O5" s="61"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="144"/>
       <c r="H6" s="65"/>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -8158,14 +8158,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="111" t="s">
+      <c r="D9" s="145" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="111"/>
-      <c r="F9" s="112" t="s">
+      <c r="E9" s="145"/>
+      <c r="F9" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="112"/>
+      <c r="G9" s="146"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -8228,14 +8228,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="112" t="s">
+      <c r="D15" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="112"/>
-      <c r="F15" s="113" t="s">
+      <c r="E15" s="146"/>
+      <c r="F15" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="113"/>
+      <c r="G15" s="147"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
gapoR - oživení výpočtů a ukládání do spojáku + kopírování do schránky + CSV + přidání tlačítka storna a souvisejících funkcionalit
TmGrid - metoda copyCells2Clipboard  + drobné fixy
vektory - univerzální metod void Text2CSV(AnsiString text,AnsiString FileName="",AnsiString Title="",AnsiString DefaultExt="",AnsiString Filter="",bool openDialog=true,bool open=true);//vytvoří a otevře CSV s daným textem, je-li požadováno
PL - uprava pro storno formu gapo_R - ještě není doladěné, bude muset dokončit Rosťa
my - AnsiString round2double(double number,unsigned short precision,AnsiString mark);//zaokrouhl� na po�et desetinn�ch m�st dle precison a vrat� hodnotu pomoc� �etezce, za ��slem n�sleduje znak, dle posledn�ho parametru (nap� dv� te�ky .. jako�e ��slo pokra�uje), pokud ��slo obsahuje re�lnou ��st nezobrazenou v r�mci precision
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -1783,63 +1783,15 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1850,6 +1802,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1858,6 +1816,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1865,60 +1865,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1933,8 +1879,62 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6967,7 +6967,7 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -7034,7 +7034,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="92" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7043,17 +7043,17 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="85"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="83"/>
+      <c r="O3" s="84"/>
       <c r="P3" s="108"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
@@ -7061,32 +7061,32 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="101"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="107"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7120,17 +7120,17 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="85"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="83"/>
+      <c r="O6" s="84"/>
       <c r="P6" s="108"/>
       <c r="R6" s="82"/>
       <c r="S6" t="s">
@@ -7138,7 +7138,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7147,17 +7147,17 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="105"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="85"/>
+      <c r="O7" s="104"/>
       <c r="P7" s="109"/>
       <c r="R7" s="2" t="s">
         <v>12</v>
@@ -7167,24 +7167,24 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="101"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="105"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="85"/>
+      <c r="O8" s="104"/>
       <c r="P8" s="109"/>
       <c r="R8" s="2" t="s">
         <v>17</v>
@@ -7194,25 +7194,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="101"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="91"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
+      <c r="P9" s="95"/>
       <c r="R9" s="71" t="s">
         <v>51</v>
       </c>
@@ -7221,24 +7221,24 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="101"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="73" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107"/>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
-      <c r="O10" s="87"/>
+      <c r="O10" s="106"/>
       <c r="P10" s="110"/>
       <c r="S10" t="s">
         <v>38</v>
@@ -7248,22 +7248,22 @@
       <c r="B11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97"/>
-      <c r="H11" s="98"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="101"/>
       <c r="I11" s="75"/>
       <c r="J11" s="77"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
       <c r="S11" t="s">
         <v>39</v>
       </c>
@@ -7295,15 +7295,17 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="G4:P4"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K11:L11"/>
@@ -7319,17 +7321,15 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7408,12 +7408,12 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="114"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="133"/>
       <c r="J3" s="80"/>
       <c r="K3" s="81"/>
       <c r="L3" s="43"/>
@@ -7442,8 +7442,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="114"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="133"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7454,42 +7454,42 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="117" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="128"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="127"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="133"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="128"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="127"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7498,20 +7498,20 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="133"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="128"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="127"/>
       <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
@@ -7520,41 +7520,41 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="111" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="120"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="119"/>
       <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="130"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="125"/>
-      <c r="M9" s="126"/>
+      <c r="D9" s="120"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="125"/>
       <c r="P9" t="s">
         <v>39</v>
       </c>
@@ -7589,14 +7589,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7613,12 +7611,14 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7632,8 +7632,8 @@
   </sheetPr>
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7655,16 +7655,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="G2" s="24" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>34</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>28</v>
@@ -7677,9 +7677,9 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="83"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="108"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
@@ -7687,7 +7687,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7705,7 +7705,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="101"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -7813,7 +7813,7 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="108"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
@@ -7821,7 +7821,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7837,7 +7837,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="101"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -7964,9 +7964,9 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="83"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="108"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
@@ -7978,7 +7978,7 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7998,7 +7998,7 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="101"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
GAPO.xlsx - fix dle PP u getTT
grafický návrh reportu - částečně využitelné (v jiných barvách a bez nadpisu) viz \DOC\graficky_navrh_reportu_obdoba.graficky_navrh_reportu_obdoba.PNG
gapoR - designové úpravy
PL - volání gapoR včetně situace okolo storna
TmGrid.cpp - oddladění chyby s posunem pozadí buněk při aktivovaném AA
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -1783,27 +1783,78 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1816,55 +1867,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1879,62 +1933,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3854,6 +3854,229 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130037</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>82393</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Obrázek 55"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4412146" y="2063613"/>
+          <a:ext cx="151138" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>131279</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83636</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>179713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Obrázek 56"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2823127" y="2062371"/>
+          <a:ext cx="151139" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>139562</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>20293</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>72869</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>163150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Obrázek 57"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="2074380"/>
+          <a:ext cx="132090" cy="142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101443</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Obrázek 58"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2443370" y="2063613"/>
+          <a:ext cx="151138" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139562</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152381" cy="171429"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Obrázek 59"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3626540" y="2062371"/>
+          <a:ext cx="152381" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>120512</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>72868</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Obrázek 60"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4005055" y="2063613"/>
+          <a:ext cx="151139" cy="171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6967,7 +7190,7 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -7034,7 +7257,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="109" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7043,50 +7266,50 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="85"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="108"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="91"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="83"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7120,25 +7343,25 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="85"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="108"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="91"/>
       <c r="R6" s="82"/>
       <c r="S6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7147,18 +7370,18 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="105"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="86"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="104"/>
-      <c r="P7" s="109"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="92"/>
       <c r="R7" s="2" t="s">
         <v>12</v>
       </c>
@@ -7167,25 +7390,25 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="83"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="105"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="104"/>
-      <c r="P8" s="109"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="92"/>
       <c r="R8" s="2" t="s">
         <v>17</v>
       </c>
@@ -7194,25 +7417,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="83"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="95"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
       <c r="R9" s="71" t="s">
         <v>51</v>
       </c>
@@ -7221,25 +7444,25 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="73" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="107"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="88"/>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="110"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="93"/>
       <c r="S10" t="s">
         <v>38</v>
       </c>
@@ -7248,22 +7471,22 @@
       <c r="B11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="96" t="s">
+      <c r="C11" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="101"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="75"/>
       <c r="J11" s="77"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="101"/>
+      <c r="O11" s="101"/>
+      <c r="P11" s="101"/>
       <c r="S11" t="s">
         <v>39</v>
       </c>
@@ -7295,18 +7518,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="E11:H11"/>
@@ -7321,15 +7541,18 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7408,12 +7631,12 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="133"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
       <c r="J3" s="80"/>
       <c r="K3" s="81"/>
       <c r="L3" s="43"/>
@@ -7442,8 +7665,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="133"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="114"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7454,42 +7677,42 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="133" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="127"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="128"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="127"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7498,20 +7721,20 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="117"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="131"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="131"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="127"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="128"/>
       <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
@@ -7520,41 +7743,41 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="129" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="118"/>
-      <c r="M8" s="119"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="120"/>
       <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="112"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="125"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="126"/>
       <c r="P9" t="s">
         <v>39</v>
       </c>
@@ -7589,12 +7812,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7611,14 +7836,12 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7632,7 +7855,7 @@
   </sheetPr>
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
@@ -7677,17 +7900,17 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="108"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="91"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7705,7 +7928,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -7813,15 +8036,15 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="108"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="91"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7837,7 +8060,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -7964,10 +8187,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="108"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="91"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -7978,7 +8201,7 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7998,7 +8221,7 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
gapoR - realizace výpočetní části
gapoV -  pouze svislá čára mezi objekty a checkboxy + textové sjednocení s gapoR
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="100">
   <si>
     <t>TT Changes</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd a jedostatečný mezerový fond</t>
+  </si>
+  <si>
+    <t>*změny proběhnou pouze v případě změny aRD a Rz (pouze v případě změny Rx,R se pro daný pohon nic neděje)</t>
   </si>
 </sst>
 </file>
@@ -1783,78 +1786,27 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1867,58 +1819,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1933,8 +1882,62 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7190,7 +7193,7 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -7257,7 +7260,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="92" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7266,50 +7269,50 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="85"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="91"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="106"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="106"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="110"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7343,25 +7346,25 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="85"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="91"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="106"/>
       <c r="R6" s="82"/>
       <c r="S6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7370,18 +7373,18 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="103"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="92"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="107"/>
       <c r="R7" s="2" t="s">
         <v>12</v>
       </c>
@@ -7390,25 +7393,25 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="106"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="103"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="92"/>
+      <c r="O8" s="102"/>
+      <c r="P8" s="107"/>
       <c r="R8" s="2" t="s">
         <v>17</v>
       </c>
@@ -7417,25 +7420,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="106"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="107"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
       <c r="R9" s="71" t="s">
         <v>51</v>
       </c>
@@ -7444,25 +7447,25 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="106"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="73" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="105"/>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="93"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="110"/>
       <c r="S10" t="s">
         <v>38</v>
       </c>
@@ -7518,15 +7521,18 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G4:P4"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="E11:H11"/>
@@ -7541,18 +7547,15 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7567,8 +7570,8 @@
   </sheetPr>
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7631,12 +7634,12 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="114"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="133"/>
       <c r="J3" s="80"/>
       <c r="K3" s="81"/>
       <c r="L3" s="43"/>
@@ -7665,8 +7668,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="114"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="133"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7677,42 +7680,42 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="117" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="128"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="127"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="133"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="128"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="127"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7721,20 +7724,20 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="133"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="128"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="127"/>
       <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
@@ -7743,48 +7746,48 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="111" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="120"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="119"/>
       <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="130"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="125"/>
-      <c r="M9" s="126"/>
+      <c r="D9" s="120"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="125"/>
       <c r="P9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
@@ -7812,14 +7815,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7836,12 +7837,14 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7900,17 +7903,17 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="91"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="106"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7928,7 +7931,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="106"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -8036,15 +8039,15 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="91"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="106"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -8060,7 +8063,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="106"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -8187,10 +8190,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="91"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="106"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -8201,7 +8204,7 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -8221,7 +8224,7 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="106"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
GAPO.xlsx - oprava - chybí zanést opravu se subskupinami R vs. Rx
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12105" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="TT" sheetId="2" r:id="rId1"/>
@@ -617,21 +617,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">aRD, RD, Rz, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> K</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="8"/>
@@ -655,6 +640,39 @@
     </r>
   </si>
   <si>
+    <t>*S&amp;G režim se zohledňuje přímo výpočtem (není možná volba), pouze ve validaci zda se stíhá přejezd</t>
+  </si>
+  <si>
+    <t>S&amp;G</t>
+  </si>
+  <si>
+    <t>není jiné volby</t>
+  </si>
+  <si>
+    <t>O8</t>
+  </si>
+  <si>
+    <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd a jedostatečný mezerový fond</t>
+  </si>
+  <si>
+    <t>*změny proběhnou pouze v případě změny aRD a Rz (pouze v případě změny Rx,R se pro daný pohon nic neděje)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aRD, RD, Rx, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> K</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -664,7 +682,7 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve">aRD, RD, Rz, </t>
+      <t xml:space="preserve">aRD, RD, Rx, </t>
     </r>
     <r>
       <rPr>
@@ -677,24 +695,6 @@
       </rPr>
       <t xml:space="preserve"> DD, CT</t>
     </r>
-  </si>
-  <si>
-    <t>*S&amp;G režim se zohledňuje přímo výpočtem (není možná volba), pouze ve validaci zda se stíhá přejezd</t>
-  </si>
-  <si>
-    <t>S&amp;G</t>
-  </si>
-  <si>
-    <t>není jiné volby</t>
-  </si>
-  <si>
-    <t>O8</t>
-  </si>
-  <si>
-    <t>*S&amp;G, PP režimy se nezohledňují, pouze ve validaci zda se stíhá přejezd a jedostatečný mezerový fond</t>
-  </si>
-  <si>
-    <t>*změny proběhnou pouze v případě změny aRD a Rz (pouze v případě změny Rx,R se pro daný pohon nic neděje)</t>
   </si>
 </sst>
 </file>
@@ -1786,27 +1786,78 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1819,55 +1870,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1882,62 +1936,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7193,8 +7193,8 @@
   </sheetPr>
   <dimension ref="B1:S16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7241,26 +7241,26 @@
         <v>77</v>
       </c>
       <c r="L2" s="76" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="M2" s="25" t="s">
         <v>80</v>
       </c>
       <c r="N2" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O2" s="52" t="s">
         <v>78</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="R2" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="109" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7269,50 +7269,50 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="85"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="106"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="91"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="83"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109"/>
+        <v>93</v>
+      </c>
+      <c r="E4" s="107"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
       <c r="R4" s="16"/>
       <c r="S4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7346,25 +7346,25 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="85"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="106"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="91"/>
       <c r="R6" s="82"/>
       <c r="S6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7373,18 +7373,18 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="103"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="86"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="107"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="92"/>
       <c r="R7" s="2" t="s">
         <v>12</v>
       </c>
@@ -7393,25 +7393,25 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="83"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="103"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="102"/>
-      <c r="P8" s="107"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="92"/>
       <c r="R8" s="2" t="s">
         <v>17</v>
       </c>
@@ -7420,25 +7420,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="83"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="109"/>
+        <v>93</v>
+      </c>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
       <c r="R9" s="71" t="s">
         <v>51</v>
       </c>
@@ -7447,25 +7447,25 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="73" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="105"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="88"/>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
-      <c r="O10" s="104"/>
-      <c r="P10" s="110"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="93"/>
       <c r="S10" t="s">
         <v>38</v>
       </c>
@@ -7501,7 +7501,7 @@
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -7521,18 +7521,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="E11:H11"/>
@@ -7547,15 +7544,18 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7570,8 +7570,8 @@
   </sheetPr>
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7634,12 +7634,12 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="133"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
       <c r="J3" s="80"/>
       <c r="K3" s="81"/>
       <c r="L3" s="43"/>
@@ -7668,8 +7668,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="133"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="114"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7680,42 +7680,42 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="133" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="102"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="127"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="128"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="127"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
       <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
@@ -7724,20 +7724,20 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="117"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="102"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="131"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="131"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="127"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="128"/>
       <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
@@ -7746,48 +7746,48 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="129" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="118"/>
-      <c r="M8" s="119"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="120"/>
       <c r="P8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="112"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="125"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="126"/>
       <c r="P9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
@@ -7815,12 +7815,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7837,14 +7839,12 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7903,17 +7903,17 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="106"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="91"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -7931,7 +7931,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -7963,7 +7963,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -8039,15 +8039,15 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="106"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="91"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -8063,7 +8063,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
@@ -8190,10 +8190,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="134"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="106"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="91"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -8204,7 +8204,7 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="106" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -8224,7 +8224,7 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
vektory -long Cvektory::vrat_pocet_objektu_bezNEBOs_prirazenymi_pohonu(bool s,short rezim) //vrátí počet objektů bez či s přiřazenými pohony (dle vstupního parametru), parametr režim ve všech režimech -1, 0 - S&G, 1-KK, 2 - PP unsigned
gapoV - aplikace výše uvedené metody, ještě však nutno ušetřit nepřiřiřazený pohon a výpis jeho parametrů
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -607,9 +607,6 @@
     <t>volba možná vždy, pokud je však z této skupiny voleno, musí být z této skupiny voleny všechny volby pro daný pohon, volby mohou být v rámci této dvouskupiny libovolné</t>
   </si>
   <si>
-    <t>pro všechny objekty se stejným pohonem  libovolnářádková volba pouze v rámci daného dvousloupce (ostatní dvousloupce jsou zakázané)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -635,7 +632,44 @@
   </si>
   <si>
     <r>
-      <t>Rz, Rx!, M, K, P</t>
+      <t xml:space="preserve">aRD, RD, R, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">  DD, CT</t>
+    </r>
+  </si>
+  <si>
+    <t>pro všechny objekty se stejným pohonem  libovolná řádková volba pouze v rámci daného dvousloupce (ostatní dvousloupce jsou zakázané)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rz, Rx!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, M, K, P</t>
     </r>
     <r>
       <rPr>
@@ -650,11 +684,51 @@
     </r>
   </si>
   <si>
-    <t>Rz,R, M, DD, P, CT</t>
-  </si>
-  <si>
     <r>
-      <t>aRD, RD, Rx,  K</t>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Rz,R,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> M, DD, P, CT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>aRD, RD, Rx</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>,  K</t>
     </r>
     <r>
       <rPr>
@@ -666,21 +740,6 @@
         <charset val="238"/>
       </rPr>
       <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">aRD, RD, R, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">  DD, CT</t>
     </r>
   </si>
 </sst>
@@ -7218,7 +7277,7 @@
   <dimension ref="B1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7262,19 +7321,19 @@
         <v>84</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L2" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>100</v>
-      </c>
       <c r="O2" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P2" s="27" t="s">
         <v>91</v>
@@ -7332,7 +7391,7 @@
       <c r="P4" s="108"/>
       <c r="R4" s="17"/>
       <c r="S4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
@@ -7357,7 +7416,7 @@
       <c r="P5" s="69"/>
       <c r="R5" s="16"/>
       <c r="S5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
@@ -7384,7 +7443,7 @@
       <c r="P6" s="106"/>
       <c r="R6" s="141"/>
       <c r="S6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TmGrid - GetIndColum, GetIndRow, HighlightRowOnMouse
</commit_message>
<xml_diff>
--- a/DOC/GAPO.xlsx
+++ b/DOC/GAPO.xlsx
@@ -1838,27 +1838,85 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1871,52 +1929,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1931,45 +2019,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2010,58 +2062,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7277,7 +7277,7 @@
   <dimension ref="B1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7343,7 +7343,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="112" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -7352,50 +7352,50 @@
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="86"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="106"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="93"/>
       <c r="R3" s="15"/>
       <c r="S3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="83"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
       <c r="R4" s="17"/>
       <c r="S4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="12" t="s">
         <v>22</v>
       </c>
@@ -7429,25 +7429,25 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="86"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="106"/>
-      <c r="R6" s="141"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="93"/>
+      <c r="R6" s="83"/>
       <c r="S6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="109" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -7456,43 +7456,43 @@
       <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="156"/>
-      <c r="N7" s="156"/>
-      <c r="O7" s="157"/>
-      <c r="P7" s="158"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="95"/>
       <c r="R7" s="82"/>
       <c r="S7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="83"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="156"/>
-      <c r="N8" s="156"/>
-      <c r="O8" s="157"/>
-      <c r="P8" s="158"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="95"/>
       <c r="R8" s="2" t="s">
         <v>12</v>
       </c>
@@ -7501,25 +7501,25 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="83"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="108"/>
-      <c r="N9" s="108"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="92"/>
       <c r="R9" s="2" t="s">
         <v>17</v>
       </c>
@@ -7528,25 +7528,25 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="73" t="s">
         <v>88</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="105"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="90"/>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
-      <c r="O10" s="104"/>
-      <c r="P10" s="109"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="96"/>
       <c r="R10" s="71" t="s">
         <v>51</v>
       </c>
@@ -7558,22 +7558,22 @@
       <c r="B11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="95"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="102"/>
       <c r="I11" s="75"/>
       <c r="J11" s="77"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="101"/>
-      <c r="P11" s="101"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="104"/>
       <c r="S11" t="s">
         <v>38</v>
       </c>
@@ -7610,18 +7610,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="G9:P9"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="G4:P4"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="E11:H11"/>
@@ -7636,15 +7633,18 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="G9:P9"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7723,12 +7723,12 @@
       <c r="C3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="126"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="117"/>
       <c r="J3" s="80"/>
       <c r="K3" s="81"/>
       <c r="L3" s="43"/>
@@ -7757,8 +7757,8 @@
       <c r="E4" s="38"/>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="126"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="117"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
       <c r="L4" s="47"/>
@@ -7769,62 +7769,62 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="144" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="102"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="122"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="145"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="132"/>
+      <c r="M5" s="133"/>
       <c r="O5" s="49"/>
       <c r="P5" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="116"/>
+      <c r="B6" s="144"/>
       <c r="C6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="146"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="144"/>
-      <c r="M6" s="145"/>
-      <c r="O6" s="141"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133"/>
+      <c r="O6" s="83"/>
       <c r="P6" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="116"/>
+      <c r="B7" s="144"/>
       <c r="C7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="102"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="148"/>
-      <c r="K7" s="149"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="145"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="136"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="133"/>
       <c r="O7" s="10" t="s">
         <v>12</v>
       </c>
@@ -7833,22 +7833,22 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="110" t="s">
+      <c r="B8" s="140" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="112"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="142"/>
-      <c r="K8" s="143"/>
-      <c r="L8" s="150"/>
-      <c r="M8" s="151"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="125"/>
       <c r="O8" s="10" t="s">
         <v>52</v>
       </c>
@@ -7857,20 +7857,20 @@
       </c>
     </row>
     <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="111"/>
+      <c r="B9" s="141"/>
       <c r="C9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="117"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="153"/>
-      <c r="L9" s="154"/>
-      <c r="M9" s="155"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="131"/>
       <c r="P9" t="s">
         <v>38</v>
       </c>
@@ -7908,12 +7908,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
@@ -7930,14 +7932,12 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7996,26 +7996,26 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="106"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="93"/>
       <c r="I3" s="15"/>
       <c r="J3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="109" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="131"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="149"/>
       <c r="I4" s="51" t="s">
         <v>12</v>
       </c>
@@ -8024,14 +8024,14 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="132"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="134"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="150"/>
+      <c r="G5" s="152"/>
       <c r="I5" s="51" t="s">
         <v>17</v>
       </c>
@@ -8040,14 +8040,14 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="128"/>
+      <c r="B6" s="146"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="137"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="155"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -8132,22 +8132,22 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="106"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="93"/>
       <c r="G3" s="15"/>
       <c r="H3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="109" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="131"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="149"/>
       <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
@@ -8156,12 +8156,12 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="132"/>
-      <c r="E5" s="134"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="152"/>
       <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
@@ -8170,12 +8170,12 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="128"/>
+      <c r="B6" s="146"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="137"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="155"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
@@ -8283,10 +8283,10 @@
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="106"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="93"/>
       <c r="H3" s="63"/>
       <c r="I3" s="58"/>
       <c r="J3" s="58"/>
@@ -8297,16 +8297,16 @@
       <c r="O3" s="61"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="109" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="131"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="149"/>
       <c r="H4" s="57"/>
       <c r="I4" s="59"/>
       <c r="J4" s="64"/>
@@ -8317,14 +8317,14 @@
       <c r="O4" s="61"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="132"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="134"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="150"/>
+      <c r="G5" s="152"/>
       <c r="H5" s="63"/>
       <c r="I5" s="59"/>
       <c r="J5" s="58"/>
@@ -8335,14 +8335,14 @@
       <c r="O5" s="61"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="128"/>
+      <c r="B6" s="146"/>
       <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="137"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="155"/>
       <c r="H6" s="65"/>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -8477,14 +8477,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="138" t="s">
+      <c r="D9" s="156" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="138"/>
-      <c r="F9" s="139" t="s">
+      <c r="E9" s="156"/>
+      <c r="F9" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="139"/>
+      <c r="G9" s="157"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -8547,14 +8547,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="139" t="s">
+      <c r="D15" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="140" t="s">
+      <c r="E15" s="157"/>
+      <c r="F15" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="140"/>
+      <c r="G15" s="158"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">

</xml_diff>